<commit_message>
get rid of active qualifer, and add red (active) bone marrow
</commit_message>
<xml_diff>
--- a/input/images/TG263_Nomenclature_to_SNOMEDCT_Codes_and_Qualifiers.xlsx
+++ b/input/images/TG263_Nomenclature_to_SNOMEDCT_Codes_and_Qualifiers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/fhir-mCODE-ig/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C302ACCF-AE2D-FD4A-8843-0825934F3C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1FFE6C-6B0E-7A42-B0DE-CE3405DD5F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="47820" windowHeight="20380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6427" uniqueCount="2552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6426" uniqueCount="2551">
   <si>
     <t>Description</t>
   </si>
@@ -7517,12 +7517,6 @@
   </si>
   <si>
     <t>438074005 | Vaginal cuff (morphologic abnormality)</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>Bone marrow structure (body structure)</t>
   </si>
   <si>
     <t>would want to double check with Chuck Mayo</t>
@@ -7730,6 +7724,9 @@
   </si>
   <si>
     <t>Ventricular System of the Brain</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Structure of red bone marrow (body structure)</t>
   </si>
 </sst>
 </file>
@@ -8804,8 +8801,8 @@
   <dimension ref="A1:U963"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A606" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I622" sqref="I622"/>
+      <pane ySplit="1" topLeftCell="A678" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K690" sqref="K690"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8853,19 +8850,19 @@
         <v>737</v>
       </c>
       <c r="K1" s="137" t="s">
-        <v>2519</v>
+        <v>2517</v>
       </c>
       <c r="L1" s="134" t="s">
-        <v>2520</v>
+        <v>2518</v>
       </c>
       <c r="M1" s="103" t="s">
-        <v>2518</v>
+        <v>2516</v>
       </c>
       <c r="N1" s="135" t="s">
-        <v>2511</v>
+        <v>2509</v>
       </c>
       <c r="O1" s="136" t="s">
-        <v>2510</v>
+        <v>2508</v>
       </c>
       <c r="P1" s="3"/>
     </row>
@@ -9675,7 +9672,7 @@
         <v>1977</v>
       </c>
       <c r="H20" s="31" t="s">
-        <v>2548</v>
+        <v>2546</v>
       </c>
       <c r="I20" s="32" t="s">
         <v>392</v>
@@ -13562,7 +13559,7 @@
       <c r="L112" s="111"/>
       <c r="M112" s="15"/>
       <c r="N112" s="161" t="s">
-        <v>2545</v>
+        <v>2543</v>
       </c>
       <c r="O112" s="26"/>
       <c r="P112" s="4"/>
@@ -18121,7 +18118,7 @@
         <v>2039</v>
       </c>
       <c r="N221" s="161" t="s">
-        <v>2541</v>
+        <v>2539</v>
       </c>
       <c r="O221" s="35" t="s">
         <v>2468</v>
@@ -19846,12 +19843,12 @@
         <v>228791009</v>
       </c>
       <c r="L262" s="111" t="s">
-        <v>2508</v>
+        <v>2506</v>
       </c>
       <c r="M262" s="15"/>
       <c r="N262" s="37"/>
       <c r="O262" s="35" t="s">
-        <v>2509</v>
+        <v>2507</v>
       </c>
       <c r="P262" s="4"/>
     </row>
@@ -19885,7 +19882,7 @@
         <v>39352004</v>
       </c>
       <c r="L263" s="76" t="s">
-        <v>2503</v>
+        <v>2501</v>
       </c>
       <c r="M263" s="12" t="s">
         <v>2465</v>
@@ -20498,14 +20495,14 @@
       <c r="J278" s="33"/>
       <c r="K278" s="145"/>
       <c r="L278" s="111" t="s">
-        <v>2507</v>
+        <v>2505</v>
       </c>
       <c r="M278" s="15"/>
       <c r="N278" s="16" t="s">
         <v>2466</v>
       </c>
       <c r="O278" s="35" t="s">
-        <v>2506</v>
+        <v>2504</v>
       </c>
       <c r="P278" s="4"/>
     </row>
@@ -20543,7 +20540,7 @@
         <v>54066008</v>
       </c>
       <c r="L279" s="76" t="s">
-        <v>2504</v>
+        <v>2502</v>
       </c>
       <c r="M279" s="49" t="s">
         <v>2467</v>
@@ -22581,7 +22578,7 @@
         <v>2067</v>
       </c>
       <c r="M328" s="15" t="s">
-        <v>2512</v>
+        <v>2510</v>
       </c>
       <c r="N328" s="37"/>
       <c r="O328" s="26"/>
@@ -22626,7 +22623,7 @@
         <v>2067</v>
       </c>
       <c r="M329" s="15" t="s">
-        <v>2513</v>
+        <v>2511</v>
       </c>
       <c r="N329" s="37"/>
       <c r="O329" s="26"/>
@@ -22671,7 +22668,7 @@
         <v>2067</v>
       </c>
       <c r="M330" s="15" t="s">
-        <v>2514</v>
+        <v>2512</v>
       </c>
       <c r="N330" s="37"/>
       <c r="O330" s="26"/>
@@ -22716,7 +22713,7 @@
         <v>2067</v>
       </c>
       <c r="M331" s="15" t="s">
-        <v>2515</v>
+        <v>2513</v>
       </c>
       <c r="N331" s="37"/>
       <c r="O331" s="26"/>
@@ -22761,7 +22758,7 @@
         <v>2067</v>
       </c>
       <c r="M332" s="15" t="s">
-        <v>2516</v>
+        <v>2514</v>
       </c>
       <c r="N332" s="37"/>
       <c r="O332" s="26"/>
@@ -22806,7 +22803,7 @@
         <v>2067</v>
       </c>
       <c r="M333" s="15" t="s">
-        <v>2517</v>
+        <v>2515</v>
       </c>
       <c r="N333" s="37"/>
       <c r="O333" s="26"/>
@@ -22927,7 +22924,7 @@
         <v>940</v>
       </c>
       <c r="I336" s="55" t="s">
-        <v>2549</v>
+        <v>2547</v>
       </c>
       <c r="J336" s="25">
         <v>233458</v>
@@ -24229,7 +24226,7 @@
         <v>127938006</v>
       </c>
       <c r="L367" s="16" t="s">
-        <v>2505</v>
+        <v>2503</v>
       </c>
       <c r="M367" s="116"/>
       <c r="N367" s="37" t="s">
@@ -24357,7 +24354,7 @@
         <v>2050</v>
       </c>
       <c r="M370" s="15" t="s">
-        <v>2522</v>
+        <v>2520</v>
       </c>
       <c r="N370" s="16"/>
       <c r="O370" s="26"/>
@@ -25600,7 +25597,7 @@
       </c>
       <c r="N398" s="118"/>
       <c r="O398" s="69" t="s">
-        <v>2521</v>
+        <v>2519</v>
       </c>
       <c r="P398" s="4"/>
     </row>
@@ -26571,10 +26568,10 @@
         <v>234280</v>
       </c>
       <c r="K423" s="138" t="s">
-        <v>2523</v>
+        <v>2521</v>
       </c>
       <c r="L423" s="76" t="s">
-        <v>2524</v>
+        <v>2522</v>
       </c>
       <c r="M423" s="15" t="s">
         <v>2039</v>
@@ -26614,10 +26611,10 @@
         <v>234280</v>
       </c>
       <c r="K424" s="138" t="s">
-        <v>2523</v>
+        <v>2521</v>
       </c>
       <c r="L424" s="76" t="s">
-        <v>2524</v>
+        <v>2522</v>
       </c>
       <c r="M424" s="15" t="s">
         <v>2040</v>
@@ -26918,13 +26915,13 @@
         <v>4719002</v>
       </c>
       <c r="L431" s="75" t="s">
+        <v>2523</v>
+      </c>
+      <c r="M431" s="15" t="s">
         <v>2525</v>
       </c>
-      <c r="M431" s="15" t="s">
-        <v>2527</v>
-      </c>
       <c r="N431" s="16" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="O431" s="26"/>
       <c r="P431" s="4"/>
@@ -26963,13 +26960,13 @@
         <v>4719002</v>
       </c>
       <c r="L432" s="75" t="s">
-        <v>2525</v>
+        <v>2523</v>
       </c>
       <c r="M432" s="15" t="s">
+        <v>2524</v>
+      </c>
+      <c r="N432" s="16" t="s">
         <v>2526</v>
-      </c>
-      <c r="N432" s="16" t="s">
-        <v>2528</v>
       </c>
       <c r="O432" s="26"/>
       <c r="P432" s="4"/>
@@ -27006,13 +27003,13 @@
         <v>4719002</v>
       </c>
       <c r="L433" s="75" t="s">
-        <v>2525</v>
+        <v>2523</v>
       </c>
       <c r="M433" s="15" t="s">
-        <v>2529</v>
+        <v>2527</v>
       </c>
       <c r="N433" s="16" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="O433" s="26"/>
       <c r="P433" s="4"/>
@@ -33238,7 +33235,7 @@
         <v>8534</v>
       </c>
       <c r="K582" s="139" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="L582" s="76" t="s">
         <v>2139</v>
@@ -33283,7 +33280,7 @@
         <v>8533</v>
       </c>
       <c r="K583" s="139" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="L583" s="76" t="s">
         <v>2139</v>
@@ -33450,7 +33447,7 @@
         <v>75093004</v>
       </c>
       <c r="L587" s="76" t="s">
-        <v>2543</v>
+        <v>2541</v>
       </c>
       <c r="M587" s="15"/>
       <c r="N587" s="16"/>
@@ -33521,10 +33518,10 @@
       </c>
       <c r="J589" s="25"/>
       <c r="K589" s="138" t="s">
-        <v>2534</v>
+        <v>2532</v>
       </c>
       <c r="L589" s="76" t="s">
-        <v>2535</v>
+        <v>2533</v>
       </c>
       <c r="M589" s="15"/>
       <c r="N589" s="86"/>
@@ -33556,10 +33553,10 @@
       <c r="I590" s="32"/>
       <c r="J590" s="33"/>
       <c r="K590" s="138" t="s">
-        <v>2536</v>
+        <v>2534</v>
       </c>
       <c r="L590" s="76" t="s">
-        <v>2537</v>
+        <v>2535</v>
       </c>
       <c r="M590" s="15"/>
       <c r="N590" s="86"/>
@@ -33634,10 +33631,10 @@
       </c>
       <c r="J592" s="25"/>
       <c r="K592" s="138" t="s">
-        <v>2538</v>
+        <v>2536</v>
       </c>
       <c r="L592" s="76" t="s">
-        <v>2539</v>
+        <v>2537</v>
       </c>
       <c r="M592" s="15"/>
       <c r="N592" s="86"/>
@@ -33678,7 +33675,7 @@
         <v>77621008</v>
       </c>
       <c r="L593" s="124" t="s">
-        <v>2540</v>
+        <v>2538</v>
       </c>
       <c r="M593" s="15" t="s">
         <v>2039</v>
@@ -33721,7 +33718,7 @@
         <v>77621008</v>
       </c>
       <c r="L594" s="124" t="s">
-        <v>2540</v>
+        <v>2538</v>
       </c>
       <c r="M594" s="15" t="s">
         <v>2040</v>
@@ -34564,10 +34561,10 @@
       </c>
       <c r="J614" s="25"/>
       <c r="K614" s="138" t="s">
-        <v>2538</v>
+        <v>2536</v>
       </c>
       <c r="L614" s="76" t="s">
-        <v>2539</v>
+        <v>2537</v>
       </c>
       <c r="M614" s="15" t="s">
         <v>2039</v>
@@ -34607,10 +34604,10 @@
       </c>
       <c r="J615" s="25"/>
       <c r="K615" s="138" t="s">
-        <v>2538</v>
+        <v>2536</v>
       </c>
       <c r="L615" s="76" t="s">
-        <v>2539</v>
+        <v>2537</v>
       </c>
       <c r="M615" s="15" t="s">
         <v>2040</v>
@@ -34747,7 +34744,7 @@
         <v>1890</v>
       </c>
       <c r="I619" s="48" t="s">
-        <v>2551</v>
+        <v>2549</v>
       </c>
       <c r="J619" s="21">
         <v>242787</v>
@@ -34756,7 +34753,7 @@
         <v>8997002</v>
       </c>
       <c r="L619" s="164" t="s">
-        <v>2550</v>
+        <v>2548</v>
       </c>
       <c r="M619" s="15"/>
       <c r="N619" s="16"/>
@@ -35257,7 +35254,7 @@
         <v>181226008</v>
       </c>
       <c r="L632" s="76" t="s">
-        <v>2542</v>
+        <v>2540</v>
       </c>
       <c r="M632" s="15"/>
       <c r="N632" s="16"/>
@@ -37089,11 +37086,11 @@
         <v>17401000</v>
       </c>
       <c r="L676" s="112" t="s">
-        <v>2547</v>
+        <v>2545</v>
       </c>
       <c r="M676" s="15"/>
       <c r="N676" s="16" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
       <c r="O676" s="35" t="s">
         <v>2468</v>
@@ -37632,7 +37629,7 @@
       <c r="L689" s="112"/>
       <c r="M689" s="15"/>
       <c r="N689" s="16" t="s">
-        <v>2544</v>
+        <v>2542</v>
       </c>
       <c r="O689" s="35" t="s">
         <v>2468</v>
@@ -37668,14 +37665,12 @@
       </c>
       <c r="J690" s="25"/>
       <c r="K690" s="138">
-        <v>14016003</v>
-      </c>
-      <c r="L690" s="76" t="s">
-        <v>2495</v>
-      </c>
-      <c r="M690" s="15" t="s">
-        <v>2494</v>
-      </c>
+        <v>75330005</v>
+      </c>
+      <c r="L690" s="164" t="s">
+        <v>2550</v>
+      </c>
+      <c r="M690" s="15"/>
       <c r="N690" s="37"/>
       <c r="O690" s="26"/>
       <c r="P690" s="4"/>
@@ -37755,7 +37750,7 @@
       </c>
       <c r="M692" s="15"/>
       <c r="N692" s="16" t="s">
-        <v>2496</v>
+        <v>2494</v>
       </c>
       <c r="O692" s="35" t="s">
         <v>2468</v>
@@ -37837,7 +37832,7 @@
         <v>1172006</v>
       </c>
       <c r="L694" s="76" t="s">
-        <v>2497</v>
+        <v>2495</v>
       </c>
       <c r="M694" s="15"/>
       <c r="N694" s="37"/>
@@ -37874,7 +37869,7 @@
         <v>79654002</v>
       </c>
       <c r="L695" s="76" t="s">
-        <v>2498</v>
+        <v>2496</v>
       </c>
       <c r="M695" s="15"/>
       <c r="N695" s="37"/>
@@ -37911,7 +37906,7 @@
         <v>123037004</v>
       </c>
       <c r="L696" s="76" t="s">
-        <v>2499</v>
+        <v>2497</v>
       </c>
       <c r="M696" s="12" t="s">
         <v>2192</v>
@@ -39343,7 +39338,7 @@
         <v>2028</v>
       </c>
       <c r="K731" s="138" t="s">
-        <v>2533</v>
+        <v>2531</v>
       </c>
       <c r="L731" s="76" t="s">
         <v>2183</v>
@@ -39393,7 +39388,7 @@
         <v>2184</v>
       </c>
       <c r="N732" s="16" t="s">
-        <v>2500</v>
+        <v>2498</v>
       </c>
       <c r="O732" s="35" t="s">
         <v>2468</v>
@@ -39431,10 +39426,10 @@
         <v>56429</v>
       </c>
       <c r="K733" s="138" t="s">
-        <v>2530</v>
+        <v>2528</v>
       </c>
       <c r="L733" s="76" t="s">
-        <v>2531</v>
+        <v>2529</v>
       </c>
       <c r="M733" s="15"/>
       <c r="N733" s="16"/>
@@ -39475,7 +39470,7 @@
         <v>35763008</v>
       </c>
       <c r="L734" s="15" t="s">
-        <v>2501</v>
+        <v>2499</v>
       </c>
       <c r="M734" s="15"/>
       <c r="N734" s="37"/>
@@ -39593,10 +39588,10 @@
         <v>2028</v>
       </c>
       <c r="K737" s="158" t="s">
-        <v>2523</v>
+        <v>2521</v>
       </c>
       <c r="L737" s="127" t="s">
-        <v>2524</v>
+        <v>2522</v>
       </c>
       <c r="M737" s="128"/>
       <c r="N737" s="16"/>
@@ -39678,7 +39673,7 @@
         <v>24999009</v>
       </c>
       <c r="L739" s="106" t="s">
-        <v>2502</v>
+        <v>2500</v>
       </c>
       <c r="M739" s="97"/>
       <c r="N739" s="37"/>
@@ -39715,7 +39710,7 @@
         <v>123037004</v>
       </c>
       <c r="L740" s="106" t="s">
-        <v>2499</v>
+        <v>2497</v>
       </c>
       <c r="M740" s="97"/>
       <c r="N740" s="37"/>

</xml_diff>

<commit_message>
added newly issued SNOMEDCT term
</commit_message>
<xml_diff>
--- a/input/images/TG263_Nomenclature_to_SNOMEDCT_Codes_and_Qualifiers.xlsx
+++ b/input/images/TG263_Nomenclature_to_SNOMEDCT_Codes_and_Qualifiers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/fhir-mCODE-ig/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30505FCB-7A85-444B-870B-A30E1606546D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75571E5A-2F3F-3142-9F75-3C3316C8C087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="500" windowWidth="56400" windowHeight="26080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2600" yWindow="500" windowWidth="56400" windowHeight="26080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapped TG263 Terms" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6470" uniqueCount="2566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6470" uniqueCount="2567">
   <si>
     <t>Description</t>
   </si>
@@ -7790,14 +7790,24 @@
   <si>
     <t>Structure of anterior descending branch of left coronary artery (body structure)</t>
   </si>
+  <si>
+    <t>USCRS-33446</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -8186,99 +8196,92 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="15" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -8286,280 +8289,288 @@
     <xf numFmtId="1" fontId="15" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -8904,9 +8915,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R903"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1:P1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A664" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K682" sqref="K682"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -16957,7 +16968,7 @@
         <v>697</v>
       </c>
       <c r="F202" s="14">
-        <f t="shared" ref="F202:F233" si="7">LEN(G202)</f>
+        <f t="shared" ref="F202:F231" si="7">LEN(G202)</f>
         <v>12</v>
       </c>
       <c r="G202" s="13" t="s">
@@ -30591,14 +30602,16 @@
         <v>1526</v>
       </c>
       <c r="J537" s="18"/>
-      <c r="K537" s="151" t="s">
-        <v>2488</v>
+      <c r="K537" s="151">
+        <v>1193554003</v>
       </c>
       <c r="L537" s="57" t="s">
         <v>2489</v>
       </c>
       <c r="M537" s="10"/>
-      <c r="N537" s="61"/>
+      <c r="N537" s="171" t="s">
+        <v>2488</v>
+      </c>
     </row>
     <row r="538" spans="1:14" s="1" customFormat="1" ht="34">
       <c r="A538" s="56"/>
@@ -35862,14 +35875,16 @@
       <c r="J673" s="26">
         <v>56429</v>
       </c>
-      <c r="K673" s="151" t="s">
-        <v>2483</v>
+      <c r="K673" s="172">
+        <v>1187337007</v>
       </c>
       <c r="L673" s="57" t="s">
         <v>2484</v>
       </c>
       <c r="M673" s="10"/>
-      <c r="N673" s="11"/>
+      <c r="N673" s="11" t="s">
+        <v>2483</v>
+      </c>
     </row>
     <row r="674" spans="1:14" s="1" customFormat="1" ht="17">
       <c r="A674" s="56"/>
@@ -36016,14 +36031,16 @@
       <c r="J677" s="67" t="s">
         <v>2026</v>
       </c>
-      <c r="K677" s="169" t="s">
-        <v>2478</v>
+      <c r="K677" s="169">
+        <v>1187336003</v>
       </c>
       <c r="L677" s="87" t="s">
         <v>2479</v>
       </c>
       <c r="M677" s="88"/>
-      <c r="N677" s="11"/>
+      <c r="N677" s="173" t="s">
+        <v>2566</v>
+      </c>
     </row>
     <row r="678" spans="1:14" s="1" customFormat="1" ht="17">
       <c r="A678" s="56"/>
@@ -39709,7 +39726,7 @@
   </sheetData>
   <autoFilter ref="A1:N680" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A55:N680">
-      <sortCondition sortBy="cellColor" ref="K1:K680" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="K1:K680" dxfId="0"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -40576,8 +40593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550FF5C6-E2A1-8B4F-8D1B-5639D9CE650F}">
   <dimension ref="A1:I159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="J40" sqref="J1:P1048576"/>
+    <sheetView topLeftCell="A33" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
added newly issued snomed codes to XLSX....forgot to do this when I added them to the Codesystem and Valueset...argh
</commit_message>
<xml_diff>
--- a/input/images/TG263_Nomenclature_to_SNOMEDCT_Codes_and_Qualifiers.xlsx
+++ b/input/images/TG263_Nomenclature_to_SNOMEDCT_Codes_and_Qualifiers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/fhir-mCODE-ig/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30505FCB-7A85-444B-870B-A30E1606546D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75571E5A-2F3F-3142-9F75-3C3316C8C087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="500" windowWidth="56400" windowHeight="26080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2600" yWindow="500" windowWidth="56400" windowHeight="26080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapped TG263 Terms" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6470" uniqueCount="2566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6470" uniqueCount="2567">
   <si>
     <t>Description</t>
   </si>
@@ -7790,14 +7790,24 @@
   <si>
     <t>Structure of anterior descending branch of left coronary artery (body structure)</t>
   </si>
+  <si>
+    <t>USCRS-33446</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -8186,99 +8196,92 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="15" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -8286,280 +8289,288 @@
     <xf numFmtId="1" fontId="15" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -8904,9 +8915,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R903"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1:P1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A664" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K682" sqref="K682"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -16957,7 +16968,7 @@
         <v>697</v>
       </c>
       <c r="F202" s="14">
-        <f t="shared" ref="F202:F233" si="7">LEN(G202)</f>
+        <f t="shared" ref="F202:F231" si="7">LEN(G202)</f>
         <v>12</v>
       </c>
       <c r="G202" s="13" t="s">
@@ -30591,14 +30602,16 @@
         <v>1526</v>
       </c>
       <c r="J537" s="18"/>
-      <c r="K537" s="151" t="s">
-        <v>2488</v>
+      <c r="K537" s="151">
+        <v>1193554003</v>
       </c>
       <c r="L537" s="57" t="s">
         <v>2489</v>
       </c>
       <c r="M537" s="10"/>
-      <c r="N537" s="61"/>
+      <c r="N537" s="171" t="s">
+        <v>2488</v>
+      </c>
     </row>
     <row r="538" spans="1:14" s="1" customFormat="1" ht="34">
       <c r="A538" s="56"/>
@@ -35862,14 +35875,16 @@
       <c r="J673" s="26">
         <v>56429</v>
       </c>
-      <c r="K673" s="151" t="s">
-        <v>2483</v>
+      <c r="K673" s="172">
+        <v>1187337007</v>
       </c>
       <c r="L673" s="57" t="s">
         <v>2484</v>
       </c>
       <c r="M673" s="10"/>
-      <c r="N673" s="11"/>
+      <c r="N673" s="11" t="s">
+        <v>2483</v>
+      </c>
     </row>
     <row r="674" spans="1:14" s="1" customFormat="1" ht="17">
       <c r="A674" s="56"/>
@@ -36016,14 +36031,16 @@
       <c r="J677" s="67" t="s">
         <v>2026</v>
       </c>
-      <c r="K677" s="169" t="s">
-        <v>2478</v>
+      <c r="K677" s="169">
+        <v>1187336003</v>
       </c>
       <c r="L677" s="87" t="s">
         <v>2479</v>
       </c>
       <c r="M677" s="88"/>
-      <c r="N677" s="11"/>
+      <c r="N677" s="173" t="s">
+        <v>2566</v>
+      </c>
     </row>
     <row r="678" spans="1:14" s="1" customFormat="1" ht="17">
       <c r="A678" s="56"/>
@@ -39709,7 +39726,7 @@
   </sheetData>
   <autoFilter ref="A1:N680" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A55:N680">
-      <sortCondition sortBy="cellColor" ref="K1:K680" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="K1:K680" dxfId="0"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -40576,8 +40593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550FF5C6-E2A1-8B4F-8D1B-5639D9CE650F}">
   <dimension ref="A1:I159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="J40" sqref="J1:P1048576"/>
+    <sheetView topLeftCell="A33" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
updated for release of SNOMED codes
</commit_message>
<xml_diff>
--- a/input/images/TG263_Nomenclature_to_SNOMEDCT_Codes_and_Qualifiers.xlsx
+++ b/input/images/TG263_Nomenclature_to_SNOMEDCT_Codes_and_Qualifiers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/fhir-mCODE-ig/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD81423-4397-5541-A370-A35C6D1A3883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C35CE9-6CCE-CC43-8D50-0B5CB21889C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2600" yWindow="500" windowWidth="56400" windowHeight="26080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7789,9 +7789,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -8187,99 +8194,92 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="16" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -8287,277 +8287,287 @@
     <xf numFmtId="1" fontId="16" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8910,8 +8920,8 @@
   <dimension ref="A1:R903"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A656" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L660" sqref="L660"/>
+      <pane ySplit="1" topLeftCell="A654" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M657" sqref="M657"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -24630,8 +24640,8 @@
       <c r="J391" s="26">
         <v>234280</v>
       </c>
-      <c r="K391" s="149" t="s">
-        <v>2478</v>
+      <c r="K391" s="149">
+        <v>1187336003</v>
       </c>
       <c r="L391" s="57" t="s">
         <v>2479</v>
@@ -24639,7 +24649,9 @@
       <c r="M391" s="10" t="s">
         <v>2037</v>
       </c>
-      <c r="N391" s="11"/>
+      <c r="N391" s="175" t="s">
+        <v>2478</v>
+      </c>
     </row>
     <row r="392" spans="1:14" s="1" customFormat="1" ht="51">
       <c r="A392" s="56" t="s">
@@ -24671,8 +24683,8 @@
       <c r="J392" s="26">
         <v>234280</v>
       </c>
-      <c r="K392" s="149" t="s">
-        <v>2478</v>
+      <c r="K392" s="149">
+        <v>1187336003</v>
       </c>
       <c r="L392" s="57" t="s">
         <v>2479</v>
@@ -24680,7 +24692,9 @@
       <c r="M392" s="10" t="s">
         <v>2038</v>
       </c>
-      <c r="N392" s="11"/>
+      <c r="N392" s="175" t="s">
+        <v>2478</v>
+      </c>
     </row>
     <row r="393" spans="1:14" s="1" customFormat="1" ht="51">
       <c r="A393" s="56" t="s">

</xml_diff>

<commit_message>
Updated to incorporate SCT codes (#268)
* play with Elixhauser questionaire

* sliced value to be boolean, Coding, or Reference(Condition)

* fixed slicing

* latest elixhauser stuff

* fixed slicing

* added overall score

* tweaked item.answer

* added issued snomed codes to replace placeholders...need to check if they are in US release

* fixed changelog

* updated for release of SNOMED codes

* Delete SD_ElixQuest.fsh

* updated notes

* Moving published SCT codes into production

* Cutting out some comments

* Correct code system urls

Co-authored-by: markkramerus <mkramer@mitre.org>
</commit_message>
<xml_diff>
--- a/input/images/TG263_Nomenclature_to_SNOMEDCT_Codes_and_Qualifiers.xlsx
+++ b/input/images/TG263_Nomenclature_to_SNOMEDCT_Codes_and_Qualifiers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/fhir-mCODE-ig/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD81423-4397-5541-A370-A35C6D1A3883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C35CE9-6CCE-CC43-8D50-0B5CB21889C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2600" yWindow="500" windowWidth="56400" windowHeight="26080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7789,9 +7789,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -8187,99 +8194,92 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="16" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -8287,277 +8287,287 @@
     <xf numFmtId="1" fontId="16" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8910,8 +8920,8 @@
   <dimension ref="A1:R903"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A656" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L660" sqref="L660"/>
+      <pane ySplit="1" topLeftCell="A654" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M657" sqref="M657"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -24630,8 +24640,8 @@
       <c r="J391" s="26">
         <v>234280</v>
       </c>
-      <c r="K391" s="149" t="s">
-        <v>2478</v>
+      <c r="K391" s="149">
+        <v>1187336003</v>
       </c>
       <c r="L391" s="57" t="s">
         <v>2479</v>
@@ -24639,7 +24649,9 @@
       <c r="M391" s="10" t="s">
         <v>2037</v>
       </c>
-      <c r="N391" s="11"/>
+      <c r="N391" s="175" t="s">
+        <v>2478</v>
+      </c>
     </row>
     <row r="392" spans="1:14" s="1" customFormat="1" ht="51">
       <c r="A392" s="56" t="s">
@@ -24671,8 +24683,8 @@
       <c r="J392" s="26">
         <v>234280</v>
       </c>
-      <c r="K392" s="149" t="s">
-        <v>2478</v>
+      <c r="K392" s="149">
+        <v>1187336003</v>
       </c>
       <c r="L392" s="57" t="s">
         <v>2479</v>
@@ -24680,7 +24692,9 @@
       <c r="M392" s="10" t="s">
         <v>2038</v>
       </c>
-      <c r="N392" s="11"/>
+      <c r="N392" s="175" t="s">
+        <v>2478</v>
+      </c>
     </row>
     <row r="393" spans="1:14" s="1" customFormat="1" ht="51">
       <c r="A393" s="56" t="s">

</xml_diff>